<commit_message>
no2. me is test
</commit_message>
<xml_diff>
--- a/omswechat0616.xlsx
+++ b/omswechat0616.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3521" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3719" uniqueCount="1414">
   <si>
     <t>步骤</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5778,6 +5778,182 @@
   </si>
   <si>
     <t>打开我的缴费记录，缴费记录中显示信息为活动信息</t>
+  </si>
+  <si>
+    <t>入口测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次登陆点击我的，验证隐私密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转后的url标题不对；社保医院变更，不对；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名显示不全，需要更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条形码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看条形码页面显示样式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四个角，右下角有一片黑的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击个人信息的入口按钮，跳转OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NoT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>认证的逻辑判断；原则内容同步数据，身份证-有身份证号码的应该都是已认证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>认证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名，身份证号，验证码非空验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有效信息录入，提交认证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交认证失败，抓包：405 Method Not Allowed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本信息:同步后需要确认个人信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步后：需要确认条形码编号正确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人业务办理，对应消息的收取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DuS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>处理中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NoDev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收缩箭头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击右侧收缩按钮可以伸展收缩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换处理中，已完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度明细查看跳转OK无误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6997,6 +7173,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -7004,6 +7185,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7022,42 +7239,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7087,17 +7268,12 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="146">
+  <dxfs count="117">
     <dxf>
       <font>
         <condense val="0"/>
@@ -7109,6 +7285,166 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -7256,27 +7592,16 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -7309,9 +7634,47 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7321,6 +7684,11 @@
         <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7338,11 +7706,42 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7379,22 +7778,16 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7409,9 +7802,14 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7421,6 +7819,11 @@
         <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7435,6 +7838,54 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -7444,7 +7895,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7465,50 +7930,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -7619,174 +8040,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8018,367 +8271,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -16087,39 +15979,39 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A356:A359 A361:A362 A2:A3 A10:A49 A85:A354">
-    <cfRule type="containsText" dxfId="145" priority="21" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="116" priority="21" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="22" operator="containsText" text="入口测试">
+    <cfRule type="containsText" dxfId="115" priority="22" operator="containsText" text="入口测试">
       <formula>NOT(ISERROR(SEARCH("入口测试",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="23" operator="containsText" text="功能测试">
+    <cfRule type="containsText" dxfId="114" priority="23" operator="containsText" text="功能测试">
       <formula>NOT(ISERROR(SEARCH("功能测试",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A49 A85:A1048576">
-    <cfRule type="cellIs" dxfId="142" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="4" operator="equal">
       <formula>"安全测试"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="20" operator="containsText" text="UI测试">
+    <cfRule type="containsText" dxfId="112" priority="20" operator="containsText" text="UI测试">
       <formula>NOT(ISERROR(SEARCH("UI测试",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98:I1048576 I1:I49 I85:I96">
-    <cfRule type="containsText" dxfId="140" priority="2" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="111" priority="2" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="110" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I343 I329:I330">
-    <cfRule type="containsText" dxfId="138" priority="5" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",I329)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I49 I85:I1048576">
-    <cfRule type="containsText" dxfId="137" priority="1" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="108" priority="1" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16205,7 +16097,7 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="72">
-      <c r="A3" s="175" t="s">
+      <c r="A3" s="173" t="s">
         <v>265</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -16230,7 +16122,7 @@
       <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="180"/>
+      <c r="A4" s="175"/>
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
@@ -16247,7 +16139,7 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="36">
-      <c r="A5" s="175" t="s">
+      <c r="A5" s="173" t="s">
         <v>266</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -16272,7 +16164,7 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="180"/>
+      <c r="A6" s="175"/>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
@@ -16289,7 +16181,7 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="48">
-      <c r="A7" s="175" t="s">
+      <c r="A7" s="173" t="s">
         <v>267</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -16310,11 +16202,11 @@
       <c r="G7" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="H7" s="164"/>
-      <c r="I7" s="182"/>
+      <c r="H7" s="167"/>
+      <c r="I7" s="170"/>
     </row>
     <row r="8" spans="1:9" ht="24">
-      <c r="A8" s="176"/>
+      <c r="A8" s="174"/>
       <c r="B8" s="7"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
@@ -16327,11 +16219,11 @@
       <c r="G8" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="H8" s="165"/>
-      <c r="I8" s="183"/>
+      <c r="H8" s="168"/>
+      <c r="I8" s="171"/>
     </row>
     <row r="9" spans="1:9" ht="24">
-      <c r="A9" s="180"/>
+      <c r="A9" s="175"/>
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
@@ -16344,11 +16236,11 @@
       <c r="G9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="166"/>
-      <c r="I9" s="184"/>
+      <c r="H9" s="169"/>
+      <c r="I9" s="172"/>
     </row>
     <row r="10" spans="1:9" ht="48">
-      <c r="A10" s="175" t="s">
+      <c r="A10" s="173" t="s">
         <v>268</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -16373,7 +16265,7 @@
       <c r="I10" s="39"/>
     </row>
     <row r="11" spans="1:9" ht="24">
-      <c r="A11" s="176"/>
+      <c r="A11" s="174"/>
       <c r="B11" s="7"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
@@ -16390,7 +16282,7 @@
       <c r="I11" s="39"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="176"/>
+      <c r="A12" s="174"/>
       <c r="B12" s="7"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
@@ -16407,7 +16299,7 @@
       <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="180"/>
+      <c r="A13" s="175"/>
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
@@ -16424,7 +16316,7 @@
       <c r="I13" s="39"/>
     </row>
     <row r="14" spans="1:9" ht="60">
-      <c r="A14" s="175" t="s">
+      <c r="A14" s="173" t="s">
         <v>269</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -16449,7 +16341,7 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="24">
-      <c r="A15" s="176"/>
+      <c r="A15" s="174"/>
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
       <c r="D15" s="15"/>
@@ -16466,7 +16358,7 @@
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="176"/>
+      <c r="A16" s="174"/>
       <c r="B16" s="7"/>
       <c r="C16" s="6"/>
       <c r="D16" s="15"/>
@@ -16483,7 +16375,7 @@
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="180"/>
+      <c r="A17" s="175"/>
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
       <c r="D17" s="15"/>
@@ -16500,7 +16392,7 @@
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="24">
-      <c r="A18" s="175" t="s">
+      <c r="A18" s="173" t="s">
         <v>270</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -16525,7 +16417,7 @@
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="180"/>
+      <c r="A19" s="175"/>
       <c r="B19" s="7"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -16542,7 +16434,7 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A20" s="173" t="s">
+      <c r="A20" s="176" t="s">
         <v>271</v>
       </c>
       <c r="B20" s="17" t="s">
@@ -16567,7 +16459,7 @@
       <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" s="20" customFormat="1">
-      <c r="A21" s="181"/>
+      <c r="A21" s="177"/>
       <c r="B21" s="17"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17"/>
@@ -16584,7 +16476,7 @@
       <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" s="20" customFormat="1">
-      <c r="A22" s="181"/>
+      <c r="A22" s="177"/>
       <c r="B22" s="17"/>
       <c r="C22" s="16"/>
       <c r="D22" s="17"/>
@@ -16601,7 +16493,7 @@
       <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" s="20" customFormat="1">
-      <c r="A23" s="181"/>
+      <c r="A23" s="177"/>
       <c r="B23" s="17"/>
       <c r="C23" s="16"/>
       <c r="D23" s="17" t="s">
@@ -16620,7 +16512,7 @@
       <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A24" s="181"/>
+      <c r="A24" s="177"/>
       <c r="B24" s="17"/>
       <c r="C24" s="16"/>
       <c r="D24" s="17" t="s">
@@ -16639,7 +16531,7 @@
       <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" s="20" customFormat="1">
-      <c r="A25" s="181"/>
+      <c r="A25" s="177"/>
       <c r="B25" s="17"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17"/>
@@ -16656,7 +16548,7 @@
       <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A26" s="181"/>
+      <c r="A26" s="177"/>
       <c r="B26" s="17"/>
       <c r="C26" s="16"/>
       <c r="D26" s="17" t="s">
@@ -16675,7 +16567,7 @@
       <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A27" s="174"/>
+      <c r="A27" s="178"/>
       <c r="B27" s="17"/>
       <c r="C27" s="16"/>
       <c r="D27" s="17" t="s">
@@ -16694,7 +16586,7 @@
       <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A28" s="173" t="s">
+      <c r="A28" s="176" t="s">
         <v>272</v>
       </c>
       <c r="B28" s="17" t="s">
@@ -16719,7 +16611,7 @@
       <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A29" s="181"/>
+      <c r="A29" s="177"/>
       <c r="B29" s="17"/>
       <c r="C29" s="16"/>
       <c r="D29" s="17" t="s">
@@ -16738,7 +16630,7 @@
       <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9" s="20" customFormat="1">
-      <c r="A30" s="181"/>
+      <c r="A30" s="177"/>
       <c r="B30" s="17"/>
       <c r="C30" s="16"/>
       <c r="D30" s="17" t="s">
@@ -16757,7 +16649,7 @@
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" s="20" customFormat="1">
-      <c r="A31" s="174"/>
+      <c r="A31" s="178"/>
       <c r="B31" s="17"/>
       <c r="C31" s="16"/>
       <c r="D31" s="17" t="s">
@@ -16776,7 +16668,7 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A32" s="173" t="s">
+      <c r="A32" s="176" t="s">
         <v>273</v>
       </c>
       <c r="B32" s="17" t="s">
@@ -16801,7 +16693,7 @@
       <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" s="20" customFormat="1" ht="24">
-      <c r="A33" s="174"/>
+      <c r="A33" s="178"/>
       <c r="B33" s="17"/>
       <c r="C33" s="16"/>
       <c r="D33" s="17" t="s">
@@ -16995,7 +16887,7 @@
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" ht="24">
-      <c r="A41" s="175" t="s">
+      <c r="A41" s="173" t="s">
         <v>281</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -17020,7 +16912,7 @@
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="176"/>
+      <c r="A42" s="174"/>
       <c r="B42" s="7"/>
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
@@ -17037,7 +16929,7 @@
       <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="176"/>
+      <c r="A43" s="174"/>
       <c r="B43" s="7"/>
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
@@ -17054,7 +16946,7 @@
       <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="176"/>
+      <c r="A44" s="174"/>
       <c r="B44" s="7"/>
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
@@ -17071,7 +16963,7 @@
       <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="176"/>
+      <c r="A45" s="174"/>
       <c r="B45" s="7"/>
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
@@ -17088,7 +16980,7 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="36">
-      <c r="A46" s="177" t="s">
+      <c r="A46" s="179" t="s">
         <v>282</v>
       </c>
       <c r="B46" s="7" t="s">
@@ -17113,7 +17005,7 @@
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="178"/>
+      <c r="A47" s="180"/>
       <c r="B47" s="7"/>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
@@ -17130,7 +17022,7 @@
       <c r="I47" s="9"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="178"/>
+      <c r="A48" s="180"/>
       <c r="B48" s="12"/>
       <c r="C48" s="11"/>
       <c r="D48" s="12"/>
@@ -17147,7 +17039,7 @@
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="178"/>
+      <c r="A49" s="180"/>
       <c r="B49" s="12"/>
       <c r="C49" s="11"/>
       <c r="D49" s="12"/>
@@ -17164,7 +17056,7 @@
       <c r="I49" s="23"/>
     </row>
     <row r="50" spans="1:9" ht="24">
-      <c r="A50" s="179"/>
+      <c r="A50" s="181"/>
       <c r="B50" s="12"/>
       <c r="C50" s="37"/>
       <c r="D50" s="7" t="s">
@@ -17183,7 +17075,7 @@
       <c r="I50" s="23"/>
     </row>
     <row r="51" spans="1:9" ht="36">
-      <c r="A51" s="164" t="s">
+      <c r="A51" s="167" t="s">
         <v>283</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -17208,7 +17100,7 @@
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="1:9" s="24" customFormat="1" ht="24">
-      <c r="A52" s="165"/>
+      <c r="A52" s="168"/>
       <c r="B52" s="7"/>
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
@@ -17225,7 +17117,7 @@
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="165"/>
+      <c r="A53" s="168"/>
       <c r="B53" s="26"/>
       <c r="C53" s="25"/>
       <c r="D53" s="26"/>
@@ -17242,7 +17134,7 @@
       <c r="I53" s="25"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="165"/>
+      <c r="A54" s="168"/>
       <c r="B54" s="7"/>
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
@@ -17259,7 +17151,7 @@
       <c r="I54" s="6"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="165"/>
+      <c r="A55" s="168"/>
       <c r="B55" s="7"/>
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
@@ -17276,7 +17168,7 @@
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="165"/>
+      <c r="A56" s="168"/>
       <c r="B56" s="7"/>
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
@@ -17293,7 +17185,7 @@
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="165"/>
+      <c r="A57" s="168"/>
       <c r="B57" s="7"/>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
@@ -17310,7 +17202,7 @@
       <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:9" ht="24">
-      <c r="A58" s="166"/>
+      <c r="A58" s="169"/>
       <c r="B58" s="7"/>
       <c r="C58" s="6"/>
       <c r="D58" s="7" t="s">
@@ -17329,7 +17221,7 @@
       <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:9" ht="24">
-      <c r="A59" s="164" t="s">
+      <c r="A59" s="167" t="s">
         <v>284</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -17354,7 +17246,7 @@
       <c r="I59" s="6"/>
     </row>
     <row r="60" spans="1:9" ht="24">
-      <c r="A60" s="165"/>
+      <c r="A60" s="168"/>
       <c r="B60" s="7"/>
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
@@ -17371,7 +17263,7 @@
       <c r="I60" s="6"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="165"/>
+      <c r="A61" s="168"/>
       <c r="B61" s="7"/>
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
@@ -17388,7 +17280,7 @@
       <c r="I61" s="6"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="165"/>
+      <c r="A62" s="168"/>
       <c r="B62" s="7"/>
       <c r="C62" s="6"/>
       <c r="D62" s="7"/>
@@ -17405,7 +17297,7 @@
       <c r="I62" s="6"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="165"/>
+      <c r="A63" s="168"/>
       <c r="B63" s="7"/>
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
@@ -17422,7 +17314,7 @@
       <c r="I63" s="6"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="165"/>
+      <c r="A64" s="168"/>
       <c r="B64" s="7"/>
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
@@ -17439,7 +17331,7 @@
       <c r="I64" s="6"/>
     </row>
     <row r="65" spans="1:9" ht="24">
-      <c r="A65" s="165"/>
+      <c r="A65" s="168"/>
       <c r="B65" s="7"/>
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
@@ -17456,7 +17348,7 @@
       <c r="I65" s="6"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="165"/>
+      <c r="A66" s="168"/>
       <c r="B66" s="7"/>
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
@@ -17473,7 +17365,7 @@
       <c r="I66" s="6"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="165"/>
+      <c r="A67" s="168"/>
       <c r="B67" s="7"/>
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
@@ -17490,7 +17382,7 @@
       <c r="I67" s="6"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="165"/>
+      <c r="A68" s="168"/>
       <c r="B68" s="7"/>
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
@@ -17507,7 +17399,7 @@
       <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="165"/>
+      <c r="A69" s="168"/>
       <c r="B69" s="7"/>
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
@@ -17524,7 +17416,7 @@
       <c r="I69" s="6"/>
     </row>
     <row r="70" spans="1:9" ht="24">
-      <c r="A70" s="165"/>
+      <c r="A70" s="168"/>
       <c r="B70" s="7"/>
       <c r="C70" s="6"/>
       <c r="D70" s="7" t="s">
@@ -17543,7 +17435,7 @@
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" ht="24">
-      <c r="A71" s="166"/>
+      <c r="A71" s="169"/>
       <c r="B71" s="7"/>
       <c r="C71" s="6"/>
       <c r="D71" s="7" t="s">
@@ -17562,7 +17454,7 @@
       <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" ht="24">
-      <c r="A72" s="164" t="s">
+      <c r="A72" s="167" t="s">
         <v>285</v>
       </c>
       <c r="B72" s="7" t="s">
@@ -17587,7 +17479,7 @@
       <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="165"/>
+      <c r="A73" s="168"/>
       <c r="B73" s="7"/>
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
@@ -17604,7 +17496,7 @@
       <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="165"/>
+      <c r="A74" s="168"/>
       <c r="B74" s="7"/>
       <c r="C74" s="6"/>
       <c r="D74" s="7"/>
@@ -17621,7 +17513,7 @@
       <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="165"/>
+      <c r="A75" s="168"/>
       <c r="B75" s="7"/>
       <c r="C75" s="6"/>
       <c r="D75" s="7"/>
@@ -17638,7 +17530,7 @@
       <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" ht="24">
-      <c r="A76" s="165"/>
+      <c r="A76" s="168"/>
       <c r="B76" s="7"/>
       <c r="C76" s="6"/>
       <c r="D76" s="7" t="s">
@@ -17657,7 +17549,7 @@
       <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="166"/>
+      <c r="A77" s="169"/>
       <c r="B77" s="7"/>
       <c r="C77" s="6"/>
       <c r="D77" s="7" t="s">
@@ -17676,7 +17568,7 @@
       <c r="I77" s="6"/>
     </row>
     <row r="78" spans="1:9" s="31" customFormat="1" ht="24">
-      <c r="A78" s="167" t="s">
+      <c r="A78" s="182" t="s">
         <v>286</v>
       </c>
       <c r="B78" s="29" t="s">
@@ -17701,7 +17593,7 @@
       <c r="I78" s="28"/>
     </row>
     <row r="79" spans="1:9" s="31" customFormat="1">
-      <c r="A79" s="168"/>
+      <c r="A79" s="183"/>
       <c r="B79" s="29"/>
       <c r="C79" s="28"/>
       <c r="D79" s="29"/>
@@ -17718,7 +17610,7 @@
       <c r="I79" s="28"/>
     </row>
     <row r="80" spans="1:9" s="31" customFormat="1">
-      <c r="A80" s="168"/>
+      <c r="A80" s="183"/>
       <c r="B80" s="29"/>
       <c r="C80" s="28"/>
       <c r="D80" s="29" t="s">
@@ -17737,7 +17629,7 @@
       <c r="I80" s="28"/>
     </row>
     <row r="81" spans="1:9" s="31" customFormat="1">
-      <c r="A81" s="168"/>
+      <c r="A81" s="183"/>
       <c r="B81" s="29"/>
       <c r="C81" s="28"/>
       <c r="D81" s="29" t="s">
@@ -17756,7 +17648,7 @@
       <c r="I81" s="28"/>
     </row>
     <row r="82" spans="1:9" s="31" customFormat="1">
-      <c r="A82" s="169"/>
+      <c r="A82" s="184"/>
       <c r="B82" s="29"/>
       <c r="C82" s="28"/>
       <c r="D82" s="29"/>
@@ -17767,7 +17659,7 @@
       <c r="I82" s="28"/>
     </row>
     <row r="83" spans="1:9" s="31" customFormat="1" ht="24">
-      <c r="A83" s="167" t="s">
+      <c r="A83" s="182" t="s">
         <v>287</v>
       </c>
       <c r="B83" s="29" t="s">
@@ -17792,7 +17684,7 @@
       <c r="I83" s="28"/>
     </row>
     <row r="84" spans="1:9" s="31" customFormat="1">
-      <c r="A84" s="168"/>
+      <c r="A84" s="183"/>
       <c r="B84" s="29"/>
       <c r="C84" s="28"/>
       <c r="D84" s="29"/>
@@ -17809,7 +17701,7 @@
       <c r="I84" s="28"/>
     </row>
     <row r="85" spans="1:9" s="31" customFormat="1">
-      <c r="A85" s="168"/>
+      <c r="A85" s="183"/>
       <c r="B85" s="29"/>
       <c r="C85" s="28"/>
       <c r="D85" s="29"/>
@@ -17826,7 +17718,7 @@
       <c r="I85" s="28"/>
     </row>
     <row r="86" spans="1:9" s="31" customFormat="1">
-      <c r="A86" s="168"/>
+      <c r="A86" s="183"/>
       <c r="B86" s="29"/>
       <c r="C86" s="28"/>
       <c r="D86" s="29"/>
@@ -17837,7 +17729,7 @@
       <c r="I86" s="28"/>
     </row>
     <row r="87" spans="1:9" s="31" customFormat="1">
-      <c r="A87" s="169"/>
+      <c r="A87" s="184"/>
       <c r="B87" s="29"/>
       <c r="C87" s="28"/>
       <c r="D87" s="29"/>
@@ -17848,7 +17740,7 @@
       <c r="I87" s="28"/>
     </row>
     <row r="88" spans="1:9" s="31" customFormat="1" ht="24">
-      <c r="A88" s="167" t="s">
+      <c r="A88" s="182" t="s">
         <v>288</v>
       </c>
       <c r="B88" s="29" t="s">
@@ -17873,7 +17765,7 @@
       <c r="I88" s="28"/>
     </row>
     <row r="89" spans="1:9" s="31" customFormat="1">
-      <c r="A89" s="168"/>
+      <c r="A89" s="183"/>
       <c r="B89" s="29"/>
       <c r="C89" s="28"/>
       <c r="D89" s="29"/>
@@ -17890,7 +17782,7 @@
       <c r="I89" s="28"/>
     </row>
     <row r="90" spans="1:9" s="31" customFormat="1">
-      <c r="A90" s="168"/>
+      <c r="A90" s="183"/>
       <c r="B90" s="29"/>
       <c r="C90" s="28"/>
       <c r="D90" s="29"/>
@@ -17907,7 +17799,7 @@
       <c r="I90" s="28"/>
     </row>
     <row r="91" spans="1:9" s="31" customFormat="1">
-      <c r="A91" s="168"/>
+      <c r="A91" s="183"/>
       <c r="B91" s="29"/>
       <c r="C91" s="28"/>
       <c r="D91" s="29"/>
@@ -17924,7 +17816,7 @@
       <c r="I91" s="28"/>
     </row>
     <row r="92" spans="1:9" s="31" customFormat="1">
-      <c r="A92" s="168"/>
+      <c r="A92" s="183"/>
       <c r="B92" s="29"/>
       <c r="C92" s="28"/>
       <c r="D92" s="29"/>
@@ -17941,7 +17833,7 @@
       <c r="I92" s="28"/>
     </row>
     <row r="93" spans="1:9" s="31" customFormat="1">
-      <c r="A93" s="168"/>
+      <c r="A93" s="183"/>
       <c r="B93" s="29"/>
       <c r="C93" s="28"/>
       <c r="D93" s="29"/>
@@ -17958,7 +17850,7 @@
       <c r="I93" s="28"/>
     </row>
     <row r="94" spans="1:9" s="31" customFormat="1">
-      <c r="A94" s="169"/>
+      <c r="A94" s="184"/>
       <c r="B94" s="29"/>
       <c r="C94" s="28"/>
       <c r="D94" s="29"/>
@@ -17969,7 +17861,7 @@
       <c r="I94" s="28"/>
     </row>
     <row r="95" spans="1:9" s="34" customFormat="1">
-      <c r="A95" s="170" t="s">
+      <c r="A95" s="185" t="s">
         <v>289</v>
       </c>
       <c r="B95" s="32" t="s">
@@ -17994,7 +17886,7 @@
       <c r="I95" s="21"/>
     </row>
     <row r="96" spans="1:9" s="34" customFormat="1">
-      <c r="A96" s="171"/>
+      <c r="A96" s="186"/>
       <c r="B96" s="32"/>
       <c r="C96" s="21"/>
       <c r="D96" s="32"/>
@@ -18011,7 +17903,7 @@
       <c r="I96" s="21"/>
     </row>
     <row r="97" spans="1:9" s="34" customFormat="1" ht="24">
-      <c r="A97" s="171"/>
+      <c r="A97" s="186"/>
       <c r="B97" s="32"/>
       <c r="C97" s="21"/>
       <c r="D97" s="32"/>
@@ -18028,7 +17920,7 @@
       <c r="I97" s="21"/>
     </row>
     <row r="98" spans="1:9" s="34" customFormat="1" ht="24">
-      <c r="A98" s="171"/>
+      <c r="A98" s="186"/>
       <c r="B98" s="32"/>
       <c r="C98" s="21"/>
       <c r="D98" s="32"/>
@@ -18045,7 +17937,7 @@
       <c r="I98" s="21"/>
     </row>
     <row r="99" spans="1:9" s="34" customFormat="1">
-      <c r="A99" s="172"/>
+      <c r="A99" s="187"/>
       <c r="B99" s="32"/>
       <c r="C99" s="21"/>
       <c r="D99" s="32"/>
@@ -18062,7 +17954,7 @@
       <c r="I99" s="21"/>
     </row>
     <row r="100" spans="1:9" s="34" customFormat="1" ht="24">
-      <c r="A100" s="170" t="s">
+      <c r="A100" s="185" t="s">
         <v>290</v>
       </c>
       <c r="B100" s="32" t="s">
@@ -18087,7 +17979,7 @@
       <c r="I100" s="21"/>
     </row>
     <row r="101" spans="1:9" s="34" customFormat="1">
-      <c r="A101" s="171"/>
+      <c r="A101" s="186"/>
       <c r="B101" s="32"/>
       <c r="C101" s="21"/>
       <c r="D101" s="32"/>
@@ -18104,7 +17996,7 @@
       <c r="I101" s="21"/>
     </row>
     <row r="102" spans="1:9" s="34" customFormat="1">
-      <c r="A102" s="171"/>
+      <c r="A102" s="186"/>
       <c r="B102" s="32"/>
       <c r="C102" s="21"/>
       <c r="D102" s="32"/>
@@ -18115,7 +18007,7 @@
       <c r="I102" s="21"/>
     </row>
     <row r="103" spans="1:9" s="34" customFormat="1">
-      <c r="A103" s="172"/>
+      <c r="A103" s="187"/>
       <c r="B103" s="32"/>
       <c r="C103" s="21"/>
       <c r="D103" s="32"/>
@@ -18126,7 +18018,7 @@
       <c r="I103" s="21"/>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="167" t="s">
         <v>291</v>
       </c>
       <c r="B104" s="7" t="s">
@@ -18151,7 +18043,7 @@
       <c r="I104" s="6"/>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="165"/>
+      <c r="A105" s="168"/>
       <c r="B105" s="7"/>
       <c r="C105" s="6"/>
       <c r="D105" s="7"/>
@@ -18168,7 +18060,7 @@
       <c r="I105" s="6"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="165"/>
+      <c r="A106" s="168"/>
       <c r="B106" s="7"/>
       <c r="C106" s="6"/>
       <c r="D106" s="7"/>
@@ -18185,7 +18077,7 @@
       <c r="I106" s="6"/>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="166"/>
+      <c r="A107" s="169"/>
       <c r="B107" s="7"/>
       <c r="C107" s="6"/>
       <c r="D107" s="7"/>
@@ -18202,7 +18094,7 @@
       <c r="I107" s="6"/>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="164" t="s">
+      <c r="A108" s="167" t="s">
         <v>292</v>
       </c>
       <c r="B108" s="7" t="s">
@@ -18227,7 +18119,7 @@
       <c r="I108" s="6"/>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="165"/>
+      <c r="A109" s="168"/>
       <c r="B109" s="7"/>
       <c r="C109" s="6"/>
       <c r="D109" s="7"/>
@@ -18244,7 +18136,7 @@
       <c r="I109" s="6"/>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="165"/>
+      <c r="A110" s="168"/>
       <c r="B110" s="7"/>
       <c r="C110" s="6"/>
       <c r="D110" s="7"/>
@@ -18261,7 +18153,7 @@
       <c r="I110" s="6"/>
     </row>
     <row r="111" spans="1:9">
-      <c r="A111" s="166"/>
+      <c r="A111" s="169"/>
       <c r="B111" s="7"/>
       <c r="C111" s="6"/>
       <c r="D111" s="7"/>
@@ -18272,7 +18164,7 @@
       <c r="I111" s="6"/>
     </row>
     <row r="112" spans="1:9" ht="24">
-      <c r="A112" s="164" t="s">
+      <c r="A112" s="167" t="s">
         <v>293</v>
       </c>
       <c r="B112" s="7" t="s">
@@ -18295,7 +18187,7 @@
       <c r="I112" s="6"/>
     </row>
     <row r="113" spans="1:9" ht="48">
-      <c r="A113" s="165"/>
+      <c r="A113" s="168"/>
       <c r="B113" s="7"/>
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
@@ -18312,7 +18204,7 @@
       <c r="I113" s="6"/>
     </row>
     <row r="114" spans="1:9" ht="24">
-      <c r="A114" s="166"/>
+      <c r="A114" s="169"/>
       <c r="B114" s="7"/>
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
@@ -24618,21 +24510,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A71"/>
     <mergeCell ref="A72:A77"/>
     <mergeCell ref="A78:A82"/>
     <mergeCell ref="A108:A111"/>
@@ -24642,6 +24519,21 @@
     <mergeCell ref="A95:A99"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A71"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24665,41 +24557,41 @@
   <sheetData>
     <row r="1" spans="4:12" ht="14.25" thickBot="1"/>
     <row r="2" spans="4:12" ht="15.75" thickTop="1" thickBot="1">
-      <c r="D2" s="185" t="s">
+      <c r="D2" s="188" t="s">
         <v>1210</v>
       </c>
-      <c r="E2" s="193"/>
-      <c r="F2" s="187"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="190"/>
       <c r="G2" s="148"/>
       <c r="H2" s="148"/>
       <c r="I2" s="148"/>
-      <c r="J2" s="185" t="s">
+      <c r="J2" s="188" t="s">
         <v>1205</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="187"/>
+      <c r="K2" s="196"/>
+      <c r="L2" s="190"/>
     </row>
     <row r="3" spans="4:12" ht="15" thickBot="1">
-      <c r="D3" s="188"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
       <c r="G3" s="149"/>
       <c r="H3" s="153"/>
       <c r="I3" s="150"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="189"/>
+      <c r="J3" s="189"/>
+      <c r="K3" s="189"/>
+      <c r="L3" s="192"/>
     </row>
     <row r="4" spans="4:12" ht="15" thickBot="1">
-      <c r="D4" s="190"/>
-      <c r="E4" s="192"/>
-      <c r="F4" s="191"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="195"/>
+      <c r="F4" s="194"/>
       <c r="G4" s="148"/>
       <c r="H4" s="148"/>
       <c r="I4" s="148"/>
-      <c r="J4" s="190"/>
-      <c r="K4" s="186"/>
-      <c r="L4" s="191"/>
+      <c r="J4" s="193"/>
+      <c r="K4" s="189"/>
+      <c r="L4" s="194"/>
     </row>
     <row r="5" spans="4:12" ht="15" thickTop="1">
       <c r="D5" s="148"/>
@@ -24730,11 +24622,11 @@
       <c r="G7" s="148"/>
       <c r="H7" s="148"/>
       <c r="I7" s="148"/>
-      <c r="J7" s="185" t="s">
+      <c r="J7" s="188" t="s">
         <v>1206</v>
       </c>
-      <c r="K7" s="186"/>
-      <c r="L7" s="187"/>
+      <c r="K7" s="189"/>
+      <c r="L7" s="190"/>
     </row>
     <row r="8" spans="4:12" ht="14.25">
       <c r="D8" s="148"/>
@@ -24743,9 +24635,9 @@
       <c r="G8" s="148"/>
       <c r="H8" s="148"/>
       <c r="I8" s="148"/>
-      <c r="J8" s="188"/>
-      <c r="K8" s="186"/>
-      <c r="L8" s="189"/>
+      <c r="J8" s="191"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="192"/>
     </row>
     <row r="9" spans="4:12" ht="15" thickBot="1">
       <c r="D9" s="148"/>
@@ -24754,9 +24646,9 @@
       <c r="G9" s="148"/>
       <c r="H9" s="148"/>
       <c r="I9" s="148"/>
-      <c r="J9" s="190"/>
-      <c r="K9" s="186"/>
-      <c r="L9" s="191"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="189"/>
+      <c r="L9" s="194"/>
     </row>
     <row r="10" spans="4:12" ht="15" thickTop="1">
       <c r="D10" s="148"/>
@@ -24787,11 +24679,11 @@
       <c r="G12" s="148"/>
       <c r="H12" s="148"/>
       <c r="I12" s="148"/>
-      <c r="J12" s="185" t="s">
+      <c r="J12" s="188" t="s">
         <v>1207</v>
       </c>
-      <c r="K12" s="186"/>
-      <c r="L12" s="187"/>
+      <c r="K12" s="189"/>
+      <c r="L12" s="190"/>
     </row>
     <row r="13" spans="4:12" ht="14.25">
       <c r="D13" s="148"/>
@@ -24800,9 +24692,9 @@
       <c r="G13" s="148"/>
       <c r="H13" s="148"/>
       <c r="I13" s="148"/>
-      <c r="J13" s="188"/>
-      <c r="K13" s="186"/>
-      <c r="L13" s="189"/>
+      <c r="J13" s="191"/>
+      <c r="K13" s="189"/>
+      <c r="L13" s="192"/>
     </row>
     <row r="14" spans="4:12" ht="15" thickBot="1">
       <c r="D14" s="148"/>
@@ -24811,9 +24703,9 @@
       <c r="G14" s="148"/>
       <c r="H14" s="148"/>
       <c r="I14" s="148"/>
-      <c r="J14" s="190"/>
-      <c r="K14" s="186"/>
-      <c r="L14" s="191"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="189"/>
+      <c r="L14" s="194"/>
     </row>
     <row r="15" spans="4:12" ht="15" thickTop="1">
       <c r="D15" s="148"/>
@@ -24838,41 +24730,41 @@
       <c r="L16" s="148"/>
     </row>
     <row r="17" spans="4:12" ht="15.75" thickTop="1" thickBot="1">
-      <c r="D17" s="185" t="s">
+      <c r="D17" s="188" t="s">
         <v>1208</v>
       </c>
-      <c r="E17" s="193"/>
-      <c r="F17" s="187"/>
+      <c r="E17" s="196"/>
+      <c r="F17" s="190"/>
       <c r="G17" s="148"/>
       <c r="H17" s="148"/>
       <c r="I17" s="148"/>
-      <c r="J17" s="185" t="s">
+      <c r="J17" s="188" t="s">
         <v>1209</v>
       </c>
-      <c r="K17" s="186"/>
-      <c r="L17" s="187"/>
+      <c r="K17" s="189"/>
+      <c r="L17" s="190"/>
     </row>
     <row r="18" spans="4:12" ht="15" thickBot="1">
-      <c r="D18" s="188"/>
-      <c r="E18" s="186"/>
-      <c r="F18" s="186"/>
+      <c r="D18" s="191"/>
+      <c r="E18" s="189"/>
+      <c r="F18" s="189"/>
       <c r="G18" s="149"/>
       <c r="H18" s="153"/>
       <c r="I18" s="150"/>
-      <c r="J18" s="186"/>
-      <c r="K18" s="186"/>
-      <c r="L18" s="189"/>
+      <c r="J18" s="189"/>
+      <c r="K18" s="189"/>
+      <c r="L18" s="192"/>
     </row>
     <row r="19" spans="4:12" ht="15" thickBot="1">
-      <c r="D19" s="190"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="191"/>
+      <c r="D19" s="193"/>
+      <c r="E19" s="195"/>
+      <c r="F19" s="194"/>
       <c r="G19" s="148"/>
       <c r="H19" s="148"/>
       <c r="I19" s="148"/>
-      <c r="J19" s="190"/>
-      <c r="K19" s="192"/>
-      <c r="L19" s="191"/>
+      <c r="J19" s="193"/>
+      <c r="K19" s="195"/>
+      <c r="L19" s="194"/>
     </row>
     <row r="20" spans="4:12" ht="14.25" thickTop="1"/>
   </sheetData>
@@ -26330,55 +26222,55 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="containsText" dxfId="136" priority="23" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="107" priority="23" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="24" operator="containsText" text="入口测试">
+    <cfRule type="containsText" dxfId="106" priority="24" operator="containsText" text="入口测试">
       <formula>NOT(ISERROR(SEARCH("入口测试",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="25" operator="containsText" text="功能测试">
+    <cfRule type="containsText" dxfId="105" priority="25" operator="containsText" text="功能测试">
       <formula>NOT(ISERROR(SEARCH("功能测试",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="cellIs" dxfId="133" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="21" operator="equal">
       <formula>"安全测试"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="22" operator="containsText" text="UI测试">
+    <cfRule type="containsText" dxfId="103" priority="22" operator="containsText" text="UI测试">
       <formula>NOT(ISERROR(SEARCH("UI测试",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K42 O3:O42">
-    <cfRule type="containsText" dxfId="131" priority="19" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="102" priority="19" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="20" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="101" priority="20" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K42 O3:O42">
-    <cfRule type="containsText" dxfId="129" priority="18" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="100" priority="18" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576 O1:O1048576">
-    <cfRule type="containsText" dxfId="128" priority="17" operator="containsText" text="NoT">
+    <cfRule type="containsText" dxfId="99" priority="17" operator="containsText" text="NoT">
       <formula>NOT(ISERROR(SEARCH("NoT",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="127" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="10" operator="equal">
       <formula>"二级模块"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="11" operator="equal">
       <formula>"其他异常"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="12" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="124" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="9" operator="equal">
       <formula>"NoDev"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29153,7 +29045,7 @@
         <v>1316</v>
       </c>
       <c r="P88" s="48"/>
-      <c r="Q88" s="194" t="s">
+      <c r="Q88" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29190,7 +29082,7 @@
         <v>1316</v>
       </c>
       <c r="P89" s="48"/>
-      <c r="Q89" s="194" t="s">
+      <c r="Q89" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29227,7 +29119,7 @@
         <v>1316</v>
       </c>
       <c r="P90" s="48"/>
-      <c r="Q90" s="194" t="s">
+      <c r="Q90" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29249,14 +29141,14 @@
       </c>
       <c r="H91" s="105"/>
       <c r="I91" s="105"/>
-      <c r="J91" s="195" t="s">
+      <c r="J91" s="165" t="s">
         <v>1359</v>
       </c>
-      <c r="K91" s="195"/>
+      <c r="K91" s="165"/>
       <c r="L91" s="105" t="s">
         <v>1303</v>
       </c>
-      <c r="M91" s="196"/>
+      <c r="M91" s="166"/>
       <c r="N91" s="137" t="s">
         <v>1360</v>
       </c>
@@ -29264,7 +29156,7 @@
         <v>1316</v>
       </c>
       <c r="P91" s="48"/>
-      <c r="Q91" s="194" t="s">
+      <c r="Q91" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29301,7 +29193,7 @@
         <v>1316</v>
       </c>
       <c r="P92" s="48"/>
-      <c r="Q92" s="194" t="s">
+      <c r="Q92" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29338,7 +29230,7 @@
         <v>1316</v>
       </c>
       <c r="P93" s="48"/>
-      <c r="Q93" s="194" t="s">
+      <c r="Q93" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29375,7 +29267,7 @@
         <v>1316</v>
       </c>
       <c r="P94" s="48"/>
-      <c r="Q94" s="194" t="s">
+      <c r="Q94" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -29404,7 +29296,7 @@
       <c r="N95" s="105"/>
       <c r="O95" s="48"/>
       <c r="P95" s="48"/>
-      <c r="Q95" s="194" t="s">
+      <c r="Q95" s="164" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -32729,120 +32621,120 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="L1 P1">
-    <cfRule type="containsText" dxfId="89" priority="46" operator="containsText" text="NoT">
+    <cfRule type="containsText" dxfId="94" priority="46" operator="containsText" text="NoT">
       <formula>NOT(ISERROR(SEARCH("NoT",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="42" operator="equal">
       <formula>"NoDev"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="87" priority="22" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="92" priority="22" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="24" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="91" priority="24" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="25" operator="containsText" text="返回测试">
+    <cfRule type="containsText" dxfId="90" priority="25" operator="containsText" text="返回测试">
       <formula>NOT(ISERROR(SEARCH("返回测试",C1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="29" operator="equal">
       <formula>"交互测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="30" operator="equal">
       <formula>"功能测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="31" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="32" operator="equal">
       <formula>"入口链接"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="33" operator="equal">
       <formula>"加载测试"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="containsText" dxfId="79" priority="19" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="84" priority="19" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="20" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="83" priority="20" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="26" operator="containsText" text="阻断">
+    <cfRule type="containsText" dxfId="82" priority="26" operator="containsText" text="阻断">
       <formula>NOT(ISERROR(SEARCH("阻断",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="27" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="81" priority="27" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="28" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="80" priority="28" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C119:C122 C70:C73">
-    <cfRule type="containsText" dxfId="74" priority="23" operator="containsText" text="交互测试1">
+    <cfRule type="containsText" dxfId="79" priority="23" operator="containsText" text="交互测试1">
       <formula>NOT(ISERROR(SEARCH("交互测试1",C70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C95">
-    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="78" priority="11" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",C88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="77" priority="12" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",C88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="13" operator="containsText" text="返回测试">
+    <cfRule type="containsText" dxfId="76" priority="13" operator="containsText" text="返回测试">
       <formula>NOT(ISERROR(SEARCH("返回测试",C88)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="14" operator="equal">
       <formula>"交互测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="15" operator="equal">
       <formula>"功能测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="16" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="17" operator="equal">
       <formula>"入口链接"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="18" operator="equal">
       <formula>"加载测试"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L89:L95">
-    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",L89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",L89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="8" operator="containsText" text="阻断">
+    <cfRule type="containsText" dxfId="68" priority="8" operator="containsText" text="阻断">
       <formula>NOT(ISERROR(SEARCH("阻断",L89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="9" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="67" priority="9" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",L89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="10" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="66" priority="10" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",L89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",L88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",L88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="阻断">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="阻断">
       <formula>NOT(ISERROR(SEARCH("阻断",L88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",L88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",L88)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33821,7 +33713,7 @@
       </c>
       <c r="N29" s="48"/>
     </row>
-    <row r="30" spans="1:15" s="47" customFormat="1" ht="36" hidden="1" outlineLevel="1">
+    <row r="30" spans="1:15" s="47" customFormat="1" ht="24" hidden="1" outlineLevel="1">
       <c r="A30" s="48"/>
       <c r="B30" s="49" t="s">
         <v>988</v>
@@ -33913,73 +33805,73 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K32 N23:N29 K25:K29 K1 O1">
-    <cfRule type="containsText" dxfId="108" priority="58" operator="containsText" text="NoT">
+    <cfRule type="containsText" dxfId="60" priority="58" operator="containsText" text="NoT">
       <formula>NOT(ISERROR(SEARCH("NoT",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32 K25:K29 K1">
-    <cfRule type="cellIs" dxfId="107" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
       <formula>"NoDev"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C1048576 C1:C22 B23:B32">
-    <cfRule type="containsText" dxfId="106" priority="49" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="58" priority="49" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="50" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="57" priority="50" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="51" operator="containsText" text="返回测试">
+    <cfRule type="containsText" dxfId="56" priority="51" operator="containsText" text="返回测试">
       <formula>NOT(ISERROR(SEARCH("返回测试",B1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="52" operator="equal">
       <formula>"交互测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="53" operator="equal">
       <formula>"功能测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
       <formula>"入口链接"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
       <formula>"加载测试"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:K1048576 L25:L32 K1:K24">
-    <cfRule type="containsText" dxfId="98" priority="44" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="50" priority="44" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="45" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="49" priority="45" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="46" operator="containsText" text="阻断">
+    <cfRule type="containsText" dxfId="48" priority="46" operator="containsText" text="阻断">
       <formula>NOT(ISERROR(SEARCH("阻断",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32 N23:N29 K25:K29">
-    <cfRule type="containsText" dxfId="93" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="22" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32 N23:N29 K25:K29">
-    <cfRule type="containsText" dxfId="91" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29 K25:K26">
-    <cfRule type="cellIs" dxfId="90" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="14" operator="equal">
       <formula>"NoDev"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33990,11 +33882,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:O122"/>
+  <dimension ref="A1:O130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -34064,100 +33956,187 @@
         <v>932</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="36">
+    <row r="2" spans="1:15">
       <c r="A2" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="48" t="s">
+        <v>1370</v>
+      </c>
       <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="D2" s="48" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I2" s="48"/>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="47" t="s">
+        <v>1376</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>1377</v>
+      </c>
+      <c r="O2" s="48"/>
+    </row>
+    <row r="3" spans="1:15" ht="24">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>1375</v>
+      </c>
+      <c r="I3" s="48"/>
+      <c r="J3" s="49" t="s">
         <v>736</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K3" s="48" t="s">
         <v>719</v>
       </c>
-      <c r="L2" s="52">
+      <c r="L3" s="52">
         <v>42895</v>
       </c>
-      <c r="M2" s="49" t="s">
-        <v>737</v>
-      </c>
-      <c r="N2" s="47" t="s">
+      <c r="M3" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="N3" s="47" t="s">
         <v>1202</v>
       </c>
-      <c r="O2" s="48"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
       <c r="O3" s="48"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="B4" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
+      <c r="J4" s="49" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>1384</v>
+      </c>
       <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
+      <c r="M4" s="48" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N4" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="O4" s="48"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="B5" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
+      <c r="J5" s="48" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K5" s="48" t="s">
+        <v>1384</v>
+      </c>
       <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
+      <c r="M5" s="48" t="s">
+        <v>1389</v>
+      </c>
+      <c r="N5" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="O5" s="48"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="48" t="s">
-        <v>846</v>
-      </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="48" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
+      <c r="J6" s="48" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>1377</v>
+      </c>
       <c r="L6" s="48"/>
       <c r="M6" s="48"/>
       <c r="N6" s="48"/>
@@ -34165,16 +34144,34 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
+      <c r="B7" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
+      <c r="J7" s="48" t="s">
+        <v>1391</v>
+      </c>
+      <c r="K7" s="48" t="s">
+        <v>1377</v>
+      </c>
       <c r="L7" s="48"/>
       <c r="M7" s="48"/>
       <c r="N7" s="48"/>
@@ -34182,86 +34179,176 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="B8" s="48" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
+      <c r="J8" s="48" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K8" s="48" t="s">
+        <v>1377</v>
+      </c>
       <c r="L8" s="48"/>
       <c r="M8" s="48"/>
       <c r="N8" s="48"/>
       <c r="O8" s="48"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="24">
       <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="B9" s="48" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
+      <c r="J9" s="48" t="s">
+        <v>1399</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>1384</v>
+      </c>
       <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
+      <c r="M9" s="49" t="s">
+        <v>1400</v>
+      </c>
+      <c r="N9" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="O9" s="48"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
+      <c r="B10" s="48" t="s">
+        <v>1397</v>
+      </c>
       <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
+      <c r="D10" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
+      <c r="J10" s="48" t="s">
+        <v>1401</v>
+      </c>
+      <c r="K10" s="48" t="s">
+        <v>1394</v>
+      </c>
       <c r="L10" s="48"/>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
       <c r="O10" s="48"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="36">
       <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
+      <c r="B11" s="48" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
+      <c r="J11" s="49" t="s">
+        <v>1395</v>
+      </c>
+      <c r="K11" s="48" t="s">
+        <v>1394</v>
+      </c>
       <c r="L11" s="48"/>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
       <c r="O11" s="48"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="48" t="s">
-        <v>847</v>
-      </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="48" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
+      <c r="J12" s="48" t="s">
+        <v>1402</v>
+      </c>
+      <c r="K12" s="48" t="s">
+        <v>1394</v>
+      </c>
       <c r="L12" s="48"/>
       <c r="M12" s="48"/>
       <c r="N12" s="48"/>
@@ -34269,33 +34356,69 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="48"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
+      <c r="B13" s="48" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
+      <c r="J13" s="48" t="s">
+        <v>1404</v>
+      </c>
+      <c r="K13" s="48" t="s">
+        <v>1405</v>
+      </c>
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
       <c r="O13" s="48"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="A14" s="48" t="s">
+        <v>846</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I14" s="48"/>
       <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
+      <c r="K14" s="48" t="s">
+        <v>1408</v>
+      </c>
       <c r="L14" s="48"/>
       <c r="M14" s="48"/>
       <c r="N14" s="48"/>
@@ -34303,16 +34426,32 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
+      <c r="B15" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I15" s="48"/>
       <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
+      <c r="K15" s="48" t="s">
+        <v>1408</v>
+      </c>
       <c r="L15" s="48"/>
       <c r="M15" s="48"/>
       <c r="N15" s="48"/>
@@ -34320,35 +34459,67 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
+      <c r="B16" s="48" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
+      <c r="J16" s="48" t="s">
+        <v>1410</v>
+      </c>
+      <c r="K16" s="48" t="s">
+        <v>1377</v>
+      </c>
       <c r="L16" s="48"/>
       <c r="M16" s="48"/>
       <c r="N16" s="48"/>
       <c r="O16" s="48"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="48" t="s">
-        <v>848</v>
-      </c>
-      <c r="B17" s="48"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48" t="s">
+        <v>1393</v>
+      </c>
       <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
+      <c r="D17" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H17" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
+      <c r="J17" s="48" t="s">
+        <v>1411</v>
+      </c>
+      <c r="K17" s="48" t="s">
+        <v>1408</v>
+      </c>
       <c r="L17" s="48"/>
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
@@ -34356,16 +34527,32 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="B18" s="48" t="s">
+        <v>1390</v>
+      </c>
       <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
+      <c r="D18" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
+      <c r="J18" s="48" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K18" s="48" t="s">
+        <v>1408</v>
+      </c>
       <c r="L18" s="48"/>
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
@@ -34373,13 +34560,25 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
+      <c r="B19" s="48" t="s">
+        <v>1413</v>
+      </c>
       <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
+      <c r="D19" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H19" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I19" s="48"/>
       <c r="J19" s="48"/>
       <c r="K19" s="48"/>
@@ -34389,14 +34588,30 @@
       <c r="O19" s="48"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
+      <c r="A20" s="48" t="s">
+        <v>847</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H20" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I20" s="48"/>
       <c r="J20" s="48"/>
       <c r="K20" s="48"/>
@@ -34407,13 +34622,27 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
+      <c r="B21" s="48" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H21" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I21" s="48"/>
       <c r="J21" s="48"/>
       <c r="K21" s="48"/>
@@ -34424,15 +34653,31 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
+      <c r="B22" s="48" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E22" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H22" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
+      <c r="J22" s="48" t="s">
+        <v>1410</v>
+      </c>
       <c r="K22" s="48"/>
       <c r="L22" s="48"/>
       <c r="M22" s="48"/>
@@ -34441,15 +34686,29 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
+      <c r="B23" s="48" t="s">
+        <v>1393</v>
+      </c>
       <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
+      <c r="D23" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H23" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
+      <c r="J23" s="48" t="s">
+        <v>1411</v>
+      </c>
       <c r="K23" s="48"/>
       <c r="L23" s="48"/>
       <c r="M23" s="48"/>
@@ -34457,18 +34716,30 @@
       <c r="O23" s="48"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="48" t="s">
-        <v>849</v>
-      </c>
-      <c r="B24" s="48"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="48" t="s">
+        <v>1390</v>
+      </c>
       <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="D24" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H24" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
+      <c r="J24" s="48" t="s">
+        <v>1412</v>
+      </c>
       <c r="K24" s="48"/>
       <c r="L24" s="48"/>
       <c r="M24" s="48"/>
@@ -34477,13 +34748,25 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
+      <c r="B25" s="48" t="s">
+        <v>1413</v>
+      </c>
       <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="D25" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F25" s="48" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G25" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H25" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="I25" s="48"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
@@ -34578,9 +34861,7 @@
       <c r="O30" s="48"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="48" t="s">
-        <v>850</v>
-      </c>
+      <c r="A31" s="48"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
@@ -34597,7 +34878,9 @@
       <c r="O31" s="48"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="48"/>
+      <c r="A32" s="48" t="s">
+        <v>849</v>
+      </c>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
@@ -34698,13 +34981,9 @@
       <c r="N37" s="48"/>
       <c r="O37" s="48"/>
     </row>
-    <row r="38" spans="1:15" ht="24">
-      <c r="A38" s="48" t="s">
-        <v>851</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>1367</v>
-      </c>
+    <row r="38" spans="1:15">
+      <c r="A38" s="48"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="48"/>
       <c r="D38" s="48"/>
       <c r="E38" s="48"/>
@@ -34712,23 +34991,17 @@
       <c r="G38" s="48"/>
       <c r="H38" s="48"/>
       <c r="I38" s="48"/>
-      <c r="J38" s="48" t="s">
-        <v>1368</v>
-      </c>
-      <c r="K38" s="48" t="s">
-        <v>1303</v>
-      </c>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
       <c r="L38" s="48"/>
-      <c r="M38" s="49" t="s">
-        <v>1369</v>
-      </c>
-      <c r="N38" s="48" t="s">
-        <v>1316</v>
-      </c>
+      <c r="M38" s="48"/>
+      <c r="N38" s="48"/>
       <c r="O38" s="48"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="48"/>
+      <c r="A39" s="48" t="s">
+        <v>850</v>
+      </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
       <c r="D39" s="48"/>
@@ -34830,9 +35103,7 @@
       <c r="O44" s="48"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="48" t="s">
-        <v>852</v>
-      </c>
+      <c r="A45" s="48"/>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>
       <c r="D45" s="48"/>
@@ -34848,9 +35119,13 @@
       <c r="N45" s="48"/>
       <c r="O45" s="48"/>
     </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
+    <row r="46" spans="1:15" ht="24">
+      <c r="A46" s="48" t="s">
+        <v>851</v>
+      </c>
+      <c r="B46" s="48" t="s">
+        <v>1367</v>
+      </c>
       <c r="C46" s="48"/>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
@@ -34858,11 +35133,19 @@
       <c r="G46" s="48"/>
       <c r="H46" s="48"/>
       <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
+      <c r="J46" s="48" t="s">
+        <v>1368</v>
+      </c>
+      <c r="K46" s="48" t="s">
+        <v>1303</v>
+      </c>
       <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
+      <c r="M46" s="49" t="s">
+        <v>1369</v>
+      </c>
+      <c r="N46" s="48" t="s">
+        <v>1316</v>
+      </c>
       <c r="O46" s="48"/>
     </row>
     <row r="47" spans="1:15">
@@ -34951,9 +35234,7 @@
       <c r="O51" s="48"/>
     </row>
     <row r="52" spans="1:15">
-      <c r="A52" s="48" t="s">
-        <v>853</v>
-      </c>
+      <c r="A52" s="48"/>
       <c r="B52" s="48"/>
       <c r="C52" s="48"/>
       <c r="D52" s="48"/>
@@ -34970,7 +35251,9 @@
       <c r="O52" s="48"/>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="48"/>
+      <c r="A53" s="48" t="s">
+        <v>852</v>
+      </c>
       <c r="B53" s="48"/>
       <c r="C53" s="48"/>
       <c r="D53" s="48"/>
@@ -35055,9 +35338,7 @@
       <c r="O57" s="48"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="48" t="s">
-        <v>854</v>
-      </c>
+      <c r="A58" s="48"/>
       <c r="B58" s="48"/>
       <c r="C58" s="48"/>
       <c r="D58" s="48"/>
@@ -35091,7 +35372,9 @@
       <c r="O59" s="48"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="48"/>
+      <c r="A60" s="48" t="s">
+        <v>853</v>
+      </c>
       <c r="B60" s="48"/>
       <c r="C60" s="48"/>
       <c r="D60" s="48"/>
@@ -35193,7 +35476,9 @@
       <c r="O65" s="48"/>
     </row>
     <row r="66" spans="1:15">
-      <c r="A66" s="48"/>
+      <c r="A66" s="48" t="s">
+        <v>854</v>
+      </c>
       <c r="B66" s="48"/>
       <c r="C66" s="48"/>
       <c r="D66" s="48"/>
@@ -36161,51 +36446,190 @@
       <c r="N122" s="48"/>
       <c r="O122" s="48"/>
     </row>
+    <row r="123" spans="1:15">
+      <c r="A123" s="48"/>
+      <c r="B123" s="48"/>
+      <c r="C123" s="48"/>
+      <c r="D123" s="48"/>
+      <c r="E123" s="48"/>
+      <c r="F123" s="48"/>
+      <c r="G123" s="48"/>
+      <c r="H123" s="48"/>
+      <c r="I123" s="48"/>
+      <c r="J123" s="48"/>
+      <c r="K123" s="48"/>
+      <c r="L123" s="48"/>
+      <c r="M123" s="48"/>
+      <c r="N123" s="48"/>
+      <c r="O123" s="48"/>
+    </row>
+    <row r="124" spans="1:15">
+      <c r="A124" s="48"/>
+      <c r="B124" s="48"/>
+      <c r="C124" s="48"/>
+      <c r="D124" s="48"/>
+      <c r="E124" s="48"/>
+      <c r="F124" s="48"/>
+      <c r="G124" s="48"/>
+      <c r="H124" s="48"/>
+      <c r="I124" s="48"/>
+      <c r="J124" s="48"/>
+      <c r="K124" s="48"/>
+      <c r="L124" s="48"/>
+      <c r="M124" s="48"/>
+      <c r="N124" s="48"/>
+      <c r="O124" s="48"/>
+    </row>
+    <row r="125" spans="1:15">
+      <c r="A125" s="48"/>
+      <c r="B125" s="48"/>
+      <c r="C125" s="48"/>
+      <c r="D125" s="48"/>
+      <c r="E125" s="48"/>
+      <c r="F125" s="48"/>
+      <c r="G125" s="48"/>
+      <c r="H125" s="48"/>
+      <c r="I125" s="48"/>
+      <c r="J125" s="48"/>
+      <c r="K125" s="48"/>
+      <c r="L125" s="48"/>
+      <c r="M125" s="48"/>
+      <c r="N125" s="48"/>
+      <c r="O125" s="48"/>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="A126" s="48"/>
+      <c r="B126" s="48"/>
+      <c r="C126" s="48"/>
+      <c r="D126" s="48"/>
+      <c r="E126" s="48"/>
+      <c r="F126" s="48"/>
+      <c r="G126" s="48"/>
+      <c r="H126" s="48"/>
+      <c r="I126" s="48"/>
+      <c r="J126" s="48"/>
+      <c r="K126" s="48"/>
+      <c r="L126" s="48"/>
+      <c r="M126" s="48"/>
+      <c r="N126" s="48"/>
+      <c r="O126" s="48"/>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="A127" s="48"/>
+      <c r="B127" s="48"/>
+      <c r="C127" s="48"/>
+      <c r="D127" s="48"/>
+      <c r="E127" s="48"/>
+      <c r="F127" s="48"/>
+      <c r="G127" s="48"/>
+      <c r="H127" s="48"/>
+      <c r="I127" s="48"/>
+      <c r="J127" s="48"/>
+      <c r="K127" s="48"/>
+      <c r="L127" s="48"/>
+      <c r="M127" s="48"/>
+      <c r="N127" s="48"/>
+      <c r="O127" s="48"/>
+    </row>
+    <row r="128" spans="1:15">
+      <c r="A128" s="48"/>
+      <c r="B128" s="48"/>
+      <c r="C128" s="48"/>
+      <c r="D128" s="48"/>
+      <c r="E128" s="48"/>
+      <c r="F128" s="48"/>
+      <c r="G128" s="48"/>
+      <c r="H128" s="48"/>
+      <c r="I128" s="48"/>
+      <c r="J128" s="48"/>
+      <c r="K128" s="48"/>
+      <c r="L128" s="48"/>
+      <c r="M128" s="48"/>
+      <c r="N128" s="48"/>
+      <c r="O128" s="48"/>
+    </row>
+    <row r="129" spans="1:15">
+      <c r="A129" s="48"/>
+      <c r="B129" s="48"/>
+      <c r="C129" s="48"/>
+      <c r="D129" s="48"/>
+      <c r="E129" s="48"/>
+      <c r="F129" s="48"/>
+      <c r="G129" s="48"/>
+      <c r="H129" s="48"/>
+      <c r="I129" s="48"/>
+      <c r="J129" s="48"/>
+      <c r="K129" s="48"/>
+      <c r="L129" s="48"/>
+      <c r="M129" s="48"/>
+      <c r="N129" s="48"/>
+      <c r="O129" s="48"/>
+    </row>
+    <row r="130" spans="1:15">
+      <c r="A130" s="48"/>
+      <c r="B130" s="48"/>
+      <c r="C130" s="48"/>
+      <c r="D130" s="48"/>
+      <c r="E130" s="48"/>
+      <c r="F130" s="48"/>
+      <c r="G130" s="48"/>
+      <c r="H130" s="48"/>
+      <c r="I130" s="48"/>
+      <c r="J130" s="48"/>
+      <c r="K130" s="48"/>
+      <c r="L130" s="48"/>
+      <c r="M130" s="48"/>
+      <c r="N130" s="48"/>
+      <c r="O130" s="48"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="K1:L1 O123:O1048576 O1:P1 K123:K1048576">
-    <cfRule type="containsText" dxfId="20" priority="37" operator="containsText" text="NoT">
+  <conditionalFormatting sqref="O131:O1048576 K131:K1048576 K1:L1 O1:P1">
+    <cfRule type="containsText" dxfId="15" priority="38" operator="containsText" text="NoT">
       <formula>NOT(ISERROR(SEARCH("NoT",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B123:B1048576 B1">
-    <cfRule type="cellIs" dxfId="19" priority="34" operator="equal">
+  <conditionalFormatting sqref="B131:B1048576 B1">
+    <cfRule type="cellIs" dxfId="14" priority="35" operator="equal">
       <formula>"二级模块"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="36" operator="equal">
       <formula>"其他异常"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="37" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:L1 K123:K1048576">
-    <cfRule type="cellIs" dxfId="16" priority="33" operator="equal">
+  <conditionalFormatting sqref="K131:K1048576 K1:L1">
+    <cfRule type="cellIs" dxfId="11" priority="34" operator="equal">
       <formula>"NoDev"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K2)))</formula>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K2)))</formula>
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K2)))</formula>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="功能">
-      <formula>NOT(ISERROR(SEARCH("功能",B1)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="入口">
+      <formula>NOT(ISERROR(SEARCH("入口",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="页面">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="链接">
+      <formula>NOT(ISERROR(SEARCH("链接",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="页面">
       <formula>NOT(ISERROR(SEARCH("页面",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="链接">
-      <formula>NOT(ISERROR(SEARCH("链接",B1)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="功能">
+      <formula>NOT(ISERROR(SEARCH("功能",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37379,65 +37803,65 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1 K1">
-    <cfRule type="containsText" dxfId="123" priority="15" operator="containsText" text="NoT">
+    <cfRule type="containsText" dxfId="41" priority="15" operator="containsText" text="NoT">
       <formula>NOT(ISERROR(SEARCH("NoT",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="122" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B23">
-    <cfRule type="containsText" dxfId="121" priority="11" operator="containsText" text="交互测试">
+    <cfRule type="containsText" dxfId="39" priority="11" operator="containsText" text="交互测试">
       <formula>NOT(ISERROR(SEARCH("交互测试",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="12" operator="containsText" text="入口测试">
+    <cfRule type="containsText" dxfId="38" priority="12" operator="containsText" text="入口测试">
       <formula>NOT(ISERROR(SEARCH("入口测试",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="13" operator="containsText" text="功能测试">
+    <cfRule type="containsText" dxfId="37" priority="13" operator="containsText" text="功能测试">
       <formula>NOT(ISERROR(SEARCH("功能测试",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B23">
-    <cfRule type="cellIs" dxfId="118" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>"安全测试"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="10" operator="containsText" text="UI测试">
+    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="UI测试">
       <formula>NOT(ISERROR(SEARCH("UI测试",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B1048576 B1:B23">
-    <cfRule type="containsText" dxfId="116" priority="5" operator="containsText" text="返回测试">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="返回测试">
       <formula>NOT(ISERROR(SEARCH("返回测试",B1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
       <formula>"页面测试"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="114" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K5">
-    <cfRule type="containsText" dxfId="112" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="4" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K5">
-    <cfRule type="containsText" dxfId="110" priority="2" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K5">
-    <cfRule type="containsText" dxfId="109" priority="1" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K4)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>